<commit_message>
dev: get credentials logic with orchestrator is done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\REF Practices\calculate_client_security_hash\calculate_client_security_hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE150B2-7005-4C64-BBCC-D52A3694F9A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE77E4DC-405D-42E3-8560-00E2ADD5263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
@@ -159,6 +159,30 @@
   </si>
   <si>
     <t>OrchestratorQueueName1</t>
+  </si>
+  <si>
+    <t>ACME_URL</t>
+  </si>
+  <si>
+    <t>SHA1_URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/login</t>
+  </si>
+  <si>
+    <t>ACME's platform</t>
+  </si>
+  <si>
+    <t>http://www.sha1-online.com/</t>
+  </si>
+  <si>
+    <t>Hash web generator</t>
+  </si>
+  <si>
+    <t>ACME_Credential</t>
+  </si>
+  <si>
+    <t>Credential for ACME's platform</t>
   </si>
 </sst>
 </file>
@@ -534,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>
@@ -602,16 +626,46 @@
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="2"/>
-    </row>
-    <row r="5" spans="1:26" ht="28.8">
-      <c r="A5" t="s">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="28.8">
+      <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -818,7 +872,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
dev: init all applications state machine is done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\REF Practices\calculate_client_security_hash\calculate_client_security_hash\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE77E4DC-405D-42E3-8560-00E2ADD5263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{891D3DC3-87D4-49ED-9592-DC6D5C9D7260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -560,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4"/>

</xml_diff>